<commit_message>
Added workflow to process all contracts in contract folder
</commit_message>
<xml_diff>
--- a/output/vendor_abcxyz_contract_extracted_contract_details.xlsx
+++ b/output/vendor_abcxyz_contract_extracted_contract_details.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,411 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
+    <col width="202" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contract Section</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Field Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Contract Title</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cloud Infrastructure Services Agreement</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Contract Reference Number</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CISA-2025-001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Contract Type</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Service Agreement</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Effective Date</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>January 1, 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Expiration Date</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>December 31, 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Contract Basics</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Contract Status</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Client Company Name</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Acme Corporation</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Client Address</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>9876 Procurement Ave, Sacramento, CA 95814</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vendor Company Name</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Vendor ABC, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Vendor Address</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1234 Cloud Street, San Francisco, CA 94105</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Primary Contact (Client)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jane Doe, Director of Procurement</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Parties Information</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Primary Contact (Vendor)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>John Smith, CEO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Financial Terms</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Total Contract Value</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$60,000 USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Financial Terms</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Payment Schedule</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Financial Terms</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Payment Terms</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Net 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Financial Terms</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Financial Terms</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Payment Method</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Terms &amp; Termination</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Termination Clause</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Either party may terminate this Agreement with thirty (30) days' written notice for any reason.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Terms &amp; Termination</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Renewal Terms</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>This Agreement shall automatically renew for successive one-year terms unless either party provides written notice of non-renewal at least thirty (30) days prior to the expiration of the current term.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Terms &amp; Termination</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Notice Period for Termination</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>30 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Terms &amp; Termination</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Notice Period for Non-Renewal</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>30 days</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Terms &amp; Termination</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Contract Duration</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>12 months</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>